<commit_message>
Add problem statement and SQL script for segregating employee data
</commit_message>
<xml_diff>
--- a/Segregate_Data/Problem_Statement.xlsx
+++ b/Segregate_Data/Problem_Statement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thoufiq/THOUFIQ/techTFQ/YouTube/VIDEOS/30 SQL Interview Queries/Video_Q4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\30DaySQLQueryChallenge - techTFQ\Segregate_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C150D3C-AD49-D048-AC2D-47ECFE4A576F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C0D2368-F221-413E-A647-C668A13998F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{316AAF8E-A88C-F84B-A155-F1A33DCE6405}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{316AAF8E-A88C-F84B-A155-F1A33DCE6405}"/>
   </bookViews>
   <sheets>
     <sheet name="Q1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
     <t>INPUT</t>
   </si>
@@ -102,7 +100,7 @@
         <rFont val="Aptos Narrow"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Query #4:</t>
+      <t>#:</t>
     </r>
     <r>
       <rPr>
@@ -115,12 +113,15 @@
       <t xml:space="preserve"> Segregate data</t>
     </r>
   </si>
+  <si>
+    <t>Rojer</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -471,23 +472,23 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -825,61 +826,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8802C92E-5D77-1E4B-A072-AA3DFA310B10}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="2" max="4" width="10.83203125" customWidth="1"/>
+    <col min="2" max="4" width="10.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="19" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:13" s="19" customFormat="1" ht="18">
+      <c r="A1" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-    </row>
-    <row r="2" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="20" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+    </row>
+    <row r="2" spans="1:13" s="19" customFormat="1">
+      <c r="B2" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-    </row>
-    <row r="3" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-    </row>
-    <row r="4" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+    </row>
+    <row r="3" spans="1:13" s="19" customFormat="1">
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+    </row>
+    <row r="4" spans="1:13" ht="16.2" thickBot="1"/>
+    <row r="5" spans="1:13" ht="16.2" thickBot="1">
       <c r="B5" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="22"/>
       <c r="D5" s="23"/>
     </row>
-    <row r="6" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="16.2" thickBot="1">
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -890,14 +891,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13">
       <c r="B7" s="4">
         <v>1</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13">
       <c r="B8" s="13">
         <v>2</v>
       </c>
@@ -906,7 +907,7 @@
       </c>
       <c r="D8" s="15"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13">
       <c r="B9" s="7">
         <v>3</v>
       </c>
@@ -915,24 +916,24 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13">
       <c r="B10" s="13">
         <v>4</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="15"/>
     </row>
-    <row r="11" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="16.2" thickBot="1">
       <c r="B11" s="10">
         <v>5</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D11" s="12"/>
     </row>
-    <row r="13" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="16.2" thickBot="1"/>
+    <row r="14" spans="1:13" ht="16.2" thickBot="1">
       <c r="B14" s="21" t="s">
         <v>6</v>
       </c>
@@ -944,7 +945,7 @@
       <c r="G14" s="22"/>
       <c r="H14" s="23"/>
     </row>
-    <row r="15" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="16.2" thickBot="1">
       <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
@@ -964,7 +965,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="16.2" thickBot="1">
       <c r="B16" s="16">
         <v>1</v>
       </c>
@@ -977,8 +978,8 @@
       <c r="F16" s="16">
         <v>5</v>
       </c>
-      <c r="G16" s="17" t="s">
-        <v>1</v>
+      <c r="G16" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="H16" s="18" t="s">
         <v>2</v>
@@ -993,5 +994,6 @@
     <mergeCell ref="A1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>